<commit_message>
remove extra fields from template. Dedupe extra fields
</commit_message>
<xml_diff>
--- a/template_input.xlsx
+++ b/template_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jas0123\curriculog_excel_sheet_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AF47DD-8069-4B9D-9538-3C929C430AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4A588C-A1D6-489F-8E86-0E84F6A83142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17304" windowHeight="8892" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="172">
   <si>
     <t>Field</t>
   </si>
@@ -165,9 +165,6 @@
     <t>AH Subcommittee</t>
   </si>
   <si>
-    <t>Banner Course Status</t>
-  </si>
-  <si>
     <t>Campus Code</t>
   </si>
   <si>
@@ -201,15 +198,6 @@
     <t>Contact Hour Distribution (if more than one instructional method)</t>
   </si>
   <si>
-    <t>Contact Hours</t>
-  </si>
-  <si>
-    <t>Course Categories (Attributes)</t>
-  </si>
-  <si>
-    <t>Course Category</t>
-  </si>
-  <si>
     <t>Course Description</t>
   </si>
   <si>
@@ -291,9 +279,6 @@
     <t>Degree Type</t>
   </si>
   <si>
-    <t>Delivery Methods</t>
-  </si>
-  <si>
     <t>Department / Division Head (Required)</t>
   </si>
   <si>
@@ -375,9 +360,6 @@
     <t>Information</t>
   </si>
   <si>
-    <t>Is Department Head review required?</t>
-  </si>
-  <si>
     <t>Is this course already approved for Variable Title or seeking Variable Title through an additional Add or Revise Course form?</t>
   </si>
   <si>
@@ -405,9 +387,6 @@
     <t>Master's Program Options</t>
   </si>
   <si>
-    <t>Max Repeat Credit</t>
-  </si>
-  <si>
     <t>Maximum Hours</t>
   </si>
   <si>
@@ -417,12 +396,6 @@
     <t>Name of Proposal</t>
   </si>
   <si>
-    <t>New / Rename Academic Unit?</t>
-  </si>
-  <si>
-    <t>New / Renamed Academic Unit Name</t>
-  </si>
-  <si>
     <t>New Academic Unit Name</t>
   </si>
   <si>
@@ -453,12 +426,6 @@
     <t>Other Catalog(s)</t>
   </si>
   <si>
-    <t>Other Grade Modes</t>
-  </si>
-  <si>
-    <t>Other Grading Scheme(s)</t>
-  </si>
-  <si>
     <t>Other Hours</t>
   </si>
   <si>
@@ -498,9 +465,6 @@
     <t>Requested Content Changes for Catalog</t>
   </si>
   <si>
-    <t>Requirement (as stated in catalog)</t>
-  </si>
-  <si>
     <t>Satisfies General Education Requirement</t>
   </si>
   <si>
@@ -516,9 +480,6 @@
     <t>Short Title (SIS)</t>
   </si>
   <si>
-    <t>Should this course be considered a Writing Emphasis course?</t>
-  </si>
-  <si>
     <t>Should this course be considered for Connections?</t>
   </si>
   <si>
@@ -571,9 +532,6 @@
   </si>
   <si>
     <t>Which committee(s) must make a decision or be informed about this submission?</t>
-  </si>
-  <si>
-    <t>Will this NEW or CHANGED/UPDATED content appear on a page that already exists?</t>
   </si>
   <si>
     <t>Will this NEW or REVISED content appear on a page that already exists?</t>
@@ -636,24 +594,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -668,28 +614,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1100,7 +1037,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1145,7 +1082,7 @@
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -1156,34 +1093,34 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1193,12 +1130,12 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1211,17 +1148,17 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1246,17 +1183,17 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
@@ -1266,12 +1203,12 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
@@ -1334,15 +1271,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A8F092-27DE-412E-8E0F-037E456B2861}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" zoomScale="86" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="94.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="94.77734375" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
@@ -1367,7 +1304,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1429,12 +1366,12 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1449,16 +1386,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1473,13 +1410,13 @@
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
@@ -1499,12 +1436,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
@@ -1518,736 +1455,661 @@
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>55</v>
+      <c r="A27" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>57</v>
+      <c r="A29" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>25</v>
+      <c r="A31" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>59</v>
+      <c r="A32" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>12</v>
+      <c r="A33" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>26</v>
+      <c r="A35" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>94</v>
+      <c r="A58" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="4" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="4" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="4" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="4" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="4" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="4" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="4" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="4" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="4" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="4" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="4" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="4" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="4" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="4" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="4" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="4" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="3" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
-        <v>138</v>
+      <c r="A106" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>139</v>
+        <v>60</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
-        <v>140</v>
+      <c r="A108" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
-        <v>142</v>
+      <c r="A110" s="4" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>143</v>
+        <v>24</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
-        <v>32</v>
+      <c r="A112" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="3" t="s">
-        <v>144</v>
+      <c r="A113" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
-        <v>145</v>
+      <c r="A114" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
-        <v>146</v>
+      <c r="A115" s="4" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="7" t="s">
-        <v>181</v>
+      <c r="A117" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="4" t="s">
-        <v>64</v>
+      <c r="A118" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
-        <v>68</v>
+      <c r="A119" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="5" t="s">
-        <v>184</v>
+      <c r="A120" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="7" t="s">
-        <v>183</v>
+      <c r="A121" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="3" t="s">
+      <c r="A124" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="3" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="3" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" s="3" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" s="3" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="3" t="s">
-        <v>161</v>
+      <c r="A140" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" s="3" t="s">
-        <v>162</v>
+      <c r="A141" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
-        <v>22</v>
+        <v>171</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" s="3" t="s">
+      <c r="A143" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" s="3" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>168</v>
+        <v>33</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165" s="3" t="s">
-        <v>179</v>
+      <c r="A150" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A179">
-    <sortCondition ref="A1:A179"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A164">
+    <sortCondition ref="A1:A164"/>
   </sortState>
-  <conditionalFormatting sqref="A18:A21">
+  <conditionalFormatting sqref="A17:A20">
     <cfRule type="duplicateValues" dxfId="8" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
+  <conditionalFormatting sqref="A21">
     <cfRule type="duplicateValues" dxfId="7" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
+  <conditionalFormatting sqref="A22">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
+  <conditionalFormatting sqref="A23">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A25:A30">
-    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
+  <conditionalFormatting sqref="A27:A36">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31:A40">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="A37:A38">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:A42">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="A52:A55">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57:A60">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="A64:A65 A67 A56:A62">
+    <cfRule type="duplicateValues" dxfId="1" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69:A70 A72 A61:A67">
-    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
+  <conditionalFormatting sqref="A24:A26">
+    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select how you want to filter data for in field. If you are using IN or BETWEEN use a comma-separated list. For BETWEEN put the lower end of your range first., e.g.: 2,5." sqref="B54" xr:uid="{FC1C90F2-4B95-448A-BDC3-18A4A56A6DFD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select how you want to filter data for in field. If you are using IN or BETWEEN use a comma-separated list. For BETWEEN put the lower end of your range first., e.g.: 2,5." sqref="B49" xr:uid="{FC1C90F2-4B95-448A-BDC3-18A4A56A6DFD}">
       <formula1>$B$4:$B$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E54" xr:uid="{FBF6BF9F-3BCF-40E3-BF58-E25772258781}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E49" xr:uid="{FBF6BF9F-3BCF-40E3-BF58-E25772258781}">
       <formula1>$A:$A</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add support for filtering by step date. Freeze template header row. Do not require separate sheets by field in final output workbook
</commit_message>
<xml_diff>
--- a/template_input.xlsx
+++ b/template_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jas0123\curriculog_excel_sheet_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4A588C-A1D6-489F-8E86-0E84F6A83142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C825A2-1F83-4588-9E0D-5E92E04CE932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t>Field</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Course Type</t>
   </si>
   <si>
-    <t>Repeat Limit</t>
-  </si>
-  <si>
     <t>Repeatability</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
     <t>GR/UG</t>
   </si>
   <si>
-    <t>High, Mid, Low</t>
-  </si>
-  <si>
     <t>NOT EQUAL TO</t>
   </si>
   <si>
@@ -303,9 +297,6 @@
     <t>Financial Impact</t>
   </si>
   <si>
-    <t>first_name</t>
-  </si>
-  <si>
     <t>flag</t>
   </si>
   <si>
@@ -553,12 +544,27 @@
   </si>
   <si>
     <t>Vol Core Categories</t>
+  </si>
+  <si>
+    <t>Proposal Launch Date Before</t>
+  </si>
+  <si>
+    <t>Current Step Started (Date)</t>
+  </si>
+  <si>
+    <t>Current Step Started Before (Date)</t>
+  </si>
+  <si>
+    <t>Current Step Started After (Date)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,21 +620,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,16 +1045,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B809DB27-F851-4238-909D-DC6D276C789A}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
@@ -1058,7 +1070,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1075,145 +1087,6 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1225,13 +1098,13 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$B$4:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B29:B292 B10:B22 B25:B27</xm:sqref>
+          <xm:sqref>B68:B292</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select the field from the proposal you want in your Excel spreadsheet._x000a_" xr:uid="{ED19FA7F-0466-4F44-81DE-819E52E3AFC1}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B28 A9:A25 A7 A2:A5</xm:sqref>
+          <xm:sqref>A2:A73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Use this to include an additional field from the proposal as a comment in the cell. Good for fields in the proposal that has lots of text.  " xr:uid="{B019C073-487B-47B8-8ABF-602FE6834B7C}">
           <x14:formula1>
@@ -1243,13 +1116,13 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>E8:E22 E1:E5 E25:E1048576</xm:sqref>
+          <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select how you want to filter data for in field. If you are using IN or BETWEEN use a comma-separated list. For BETWEEN put the lower end of your range first., e.g.: 2,5." xr:uid="{FEA64857-E951-453F-B873-F85426215CF0}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$B:$B</xm:f>
           </x14:formula1>
-          <xm:sqref>B7 B2 B4:B5</xm:sqref>
+          <xm:sqref>B2:B67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field to separate sheets by. Creates a separate sheet for each unique value in the field. If the field is &quot;College&quot; and the proposals are from A&amp;S and Tickle Engineering, a sheet titled A&amp;S and a sheet titled Tickle Engineering are created." xr:uid="{CCE53851-1D4A-4889-8217-59A49DFAA977}">
           <x14:formula1>
@@ -1261,7 +1134,7 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$E:$E</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F4</xm:sqref>
+          <xm:sqref>F2:F22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1271,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A8F092-27DE-412E-8E0F-037E456B2861}">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView topLeftCell="A131" zoomScale="86" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1304,7 +1177,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1366,12 +1239,12 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1386,7 +1259,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1436,7 +1309,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
@@ -1481,22 +1354,22 @@
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
@@ -1510,573 +1383,588 @@
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>78</v>
+      <c r="A38" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>79</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>166</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>63</v>
+      <c r="A48" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>87</v>
+      <c r="A51" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>89</v>
+      <c r="A53" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>90</v>
+      <c r="A54" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>68</v>
+      <c r="A58" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>59</v>
+      <c r="A67" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
-        <v>102</v>
+      <c r="A69" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
-        <v>32</v>
+      <c r="A101" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="s">
-        <v>134</v>
+      <c r="A103" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
-        <v>73</v>
+      <c r="A105" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>64</v>
+      <c r="A108" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="4" t="s">
-        <v>169</v>
+      <c r="A110" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
-        <v>24</v>
+      <c r="A111" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>11</v>
+        <v>167</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="4" t="s">
-        <v>137</v>
+      <c r="A114" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
-        <v>138</v>
+      <c r="A115" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
-        <v>58</v>
+      <c r="A118" s="4" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
-        <v>143</v>
+      <c r="A121" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="3" t="s">
-        <v>22</v>
+      <c r="A128" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="5" t="s">
-        <v>62</v>
+      <c r="A130" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="4" t="s">
-        <v>151</v>
+      <c r="A131" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="4" t="s">
-        <v>153</v>
+      <c r="A133" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="2" t="s">
-        <v>61</v>
+      <c r="A136" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="5" t="s">
-        <v>66</v>
+      <c r="A137" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="3" t="s">
-        <v>23</v>
+      <c r="A139" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="4" t="s">
-        <v>157</v>
+      <c r="A140" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" s="4" t="s">
-        <v>171</v>
+      <c r="A142" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" s="3" t="s">
-        <v>33</v>
+      <c r="A149" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A164">
-    <sortCondition ref="A1:A164"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A153">
+    <sortCondition ref="A1:A153"/>
   </sortState>
   <conditionalFormatting sqref="A17:A20">
     <cfRule type="duplicateValues" dxfId="8" priority="13"/>
@@ -2090,20 +1978,20 @@
   <conditionalFormatting sqref="A23">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A24:A26">
+    <cfRule type="duplicateValues" dxfId="4" priority="18"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A27:A36">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:A38">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52:A55">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="A52:A54">
+    <cfRule type="duplicateValues" dxfId="1" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A64:A65 A67 A56:A62">
-    <cfRule type="duplicateValues" dxfId="1" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24:A26">
-    <cfRule type="duplicateValues" dxfId="0" priority="18"/>
+  <conditionalFormatting sqref="A63:A64 A66 A55:A61">
+    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select how you want to filter data for in field. If you are using IN or BETWEEN use a comma-separated list. For BETWEEN put the lower end of your range first., e.g.: 2,5." sqref="B49" xr:uid="{FC1C90F2-4B95-448A-BDC3-18A4A56A6DFD}">

</xml_diff>

<commit_message>
update template. allow ignoring fields used to filter data. Transform college names to shortened names.
</commit_message>
<xml_diff>
--- a/template_input.xlsx
+++ b/template_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jspenc35\curriculog_excel_sheet_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A4D5C0-95B8-45BC-B6A9-61DBB5A03806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5033666-E1EC-4796-BA49-01F4A4942185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="175">
   <si>
     <t>Field</t>
   </si>
@@ -556,6 +556,12 @@
   </si>
   <si>
     <t>Current Step Started After (Date)</t>
+  </si>
+  <si>
+    <t>UG Curriculum Committee</t>
+  </si>
+  <si>
+    <t>Don't Return Field</t>
   </si>
 </sst>
 </file>
@@ -749,9 +755,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -789,7 +795,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -895,7 +901,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1037,7 +1043,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1045,25 +1051,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B809DB27-F851-4238-909D-DC6D276C789A}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1073,45 +1080,85 @@
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8">
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1135,13 +1182,13 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>D9:D20 D2:D6</xm:sqref>
+          <xm:sqref>E9:E20 E2:E6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FBF6BF9F-3BCF-40E3-BF58-E25772258781}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select how you want to filter data for in field. If you are using IN or BETWEEN use a comma-separated list. For BETWEEN put the lower end of your range first., e.g.: 2,5." xr:uid="{FEA64857-E951-453F-B873-F85426215CF0}">
           <x14:formula1>
@@ -1153,13 +1200,13 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H6 H8</xm:sqref>
+          <xm:sqref>I2:I6 I8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A32929B-C51D-4A5A-BFA3-4B20B2A647A4}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$E:$E</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F23</xm:sqref>
+          <xm:sqref>G2:G23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1175,18 +1222,18 @@
       <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="94.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -1197,7 +1244,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1208,7 +1255,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1219,7 +1266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -1227,7 +1274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -1235,7 +1282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1243,7 +1290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -1251,7 +1298,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
@@ -1259,7 +1306,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -1267,722 +1314,722 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="4" t="s">
         <v>162</v>
       </c>

</xml_diff>

<commit_message>
Add embedding proposal URL to field.
</commit_message>
<xml_diff>
--- a/template_input.xlsx
+++ b/template_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jspenc35\curriculog_excel_sheet_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5033666-E1EC-4796-BA49-01F4A4942185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA82363-312D-4B52-9E3D-35DDBEBA7BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{125E1219-2066-4676-87E7-42C796F6CDDF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="176">
   <si>
     <t>Field</t>
   </si>
@@ -562,6 +562,9 @@
   </si>
   <si>
     <t>Don't Return Field</t>
+  </si>
+  <si>
+    <t>Embed URL</t>
   </si>
 </sst>
 </file>
@@ -1051,26 +1054,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B809DB27-F851-4238-909D-DC6D276C789A}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.54296875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1081,36 +1084,39 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1120,11 +1126,11 @@
       <c r="C3" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="8" t="b">
+      <c r="E3" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -1135,28 +1141,31 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>59</v>
       </c>
-      <c r="F5" t="s">
+      <c r="D5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>59</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1182,13 +1191,13 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>E9:E20 E2:E6</xm:sqref>
+          <xm:sqref>F9:F20 F2:F6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FBF6BF9F-3BCF-40E3-BF58-E25772258781}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
+          <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select how you want to filter data for in field. If you are using IN or BETWEEN use a comma-separated list. For BETWEEN put the lower end of your range first., e.g.: 2,5." xr:uid="{FEA64857-E951-453F-B873-F85426215CF0}">
           <x14:formula1>
@@ -1200,13 +1209,13 @@
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I6 I8</xm:sqref>
+          <xm:sqref>J2:J6 J8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A32929B-C51D-4A5A-BFA3-4B20B2A647A4}">
           <x14:formula1>
             <xm:f>'Options (Ignore)'!$E:$E</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G23</xm:sqref>
+          <xm:sqref>H2:H23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>